<commit_message>
added basic card responsiveness
</commit_message>
<xml_diff>
--- a/server/brokerage_data.xlsx
+++ b/server/brokerage_data.xlsx
@@ -1,17 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26215"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tanooj/dynamic_UI/server/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="9495" windowHeight="6165"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="24460" windowHeight="17280"/>
   </bookViews>
   <sheets>
     <sheet name="member_profiles" sheetId="1" r:id="rId1"/>
     <sheet name="kmp" sheetId="2" r:id="rId2"/>
     <sheet name="authorized_personnel" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -630,11 +640,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -737,6 +747,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -783,7 +798,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -815,9 +830,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -849,6 +865,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1024,20 +1041,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1054,7 +1071,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="3" customFormat="1">
+    <row r="2" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>13233</v>
       </c>
@@ -1071,7 +1088,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="3" customFormat="1">
+    <row r="3" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>9098</v>
       </c>
@@ -1088,7 +1105,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="3" customFormat="1">
+    <row r="4" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>90039</v>
       </c>
@@ -1105,7 +1122,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="3" customFormat="1">
+    <row r="5" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>6430</v>
       </c>
@@ -1122,7 +1139,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="3" customFormat="1">
+    <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>12965</v>
       </c>
@@ -1139,7 +1156,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="3" customFormat="1">
+    <row r="7" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>7701</v>
       </c>
@@ -1156,7 +1173,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="3" customFormat="1">
+    <row r="8" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>6962</v>
       </c>
@@ -1173,7 +1190,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="3" customFormat="1">
+    <row r="9" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>8854</v>
       </c>
@@ -1190,7 +1207,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="3" customFormat="1">
+    <row r="10" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>8256</v>
       </c>
@@ -1207,7 +1224,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="3" customFormat="1">
+    <row r="11" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>90135</v>
       </c>
@@ -1231,25 +1248,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="2" max="2" width="25.5" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="0" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" customWidth="1"/>
-    <col min="8" max="8" width="34.42578125" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" customWidth="1"/>
+    <col min="8" max="8" width="34.5" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1278,7 +1295,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -1307,7 +1324,7 @@
         <v>39954</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1336,7 +1353,7 @@
         <v>41341</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -1365,7 +1382,7 @@
         <v>39263</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -1394,7 +1411,7 @@
         <v>42771</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -1423,7 +1440,7 @@
         <v>39703</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1452,7 +1469,7 @@
         <v>36434</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -1481,7 +1498,7 @@
         <v>40645</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -1510,7 +1527,7 @@
         <v>42233</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -1539,7 +1556,7 @@
         <v>37518</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -1568,7 +1585,7 @@
         <v>38879</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>48</v>
       </c>
@@ -1597,7 +1614,7 @@
         <v>38032</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>56</v>
       </c>
@@ -1626,7 +1643,7 @@
         <v>43814</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="30">
+    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>61</v>
       </c>
@@ -1655,7 +1672,7 @@
         <v>40187</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="39">
+    <row r="15" spans="1:9" ht="40" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>61</v>
       </c>
@@ -1684,7 +1701,7 @@
         <v>40915</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>67</v>
       </c>
@@ -1713,7 +1730,7 @@
         <v>38961</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>67</v>
       </c>
@@ -1742,7 +1759,7 @@
         <v>41644</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>73</v>
       </c>
@@ -1771,7 +1788,7 @@
         <v>42373</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>73</v>
       </c>
@@ -1826,21 +1843,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S12" sqref="S12"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.5" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1869,7 +1886,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -1898,7 +1915,7 @@
         <v>40421</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>20</v>
       </c>
@@ -1927,7 +1944,7 @@
         <v>41061</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
         <v>29</v>
       </c>
@@ -1956,7 +1973,7 @@
         <v>40162</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
         <v>36</v>
       </c>
@@ -1985,7 +2002,7 @@
         <v>39918</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>41</v>
       </c>
@@ -2014,7 +2031,7 @@
         <v>38353</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>48</v>
       </c>
@@ -2043,7 +2060,7 @@
         <v>42139</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
         <v>56</v>
       </c>
@@ -2072,7 +2089,7 @@
         <v>38763</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>61</v>
       </c>
@@ -2101,7 +2118,7 @@
         <v>43282</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
         <v>132</v>
       </c>
@@ -2130,7 +2147,7 @@
         <v>38078</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>73</v>
       </c>

</xml_diff>

<commit_message>
added some styling for d3 graph
</commit_message>
<xml_diff>
--- a/server/brokerage_data.xlsx
+++ b/server/brokerage_data.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26215"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tanooj/dynamic_UI/server/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="24460" windowHeight="17280"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="member_profiles" sheetId="1" r:id="rId1"/>
@@ -28,9 +23,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="203">
   <si>
-    <t>Member ID</t>
-  </si>
-  <si>
     <t>Segments</t>
   </si>
   <si>
@@ -46,9 +38,6 @@
     <t>Capital Market,Capital Market,Currency Futures,Futures &amp; Options,Futures &amp; Options, IPO</t>
   </si>
   <si>
-    <t>SEBI Registration No</t>
-  </si>
-  <si>
     <t>406 Grand Mall, Opp SBI Zonal Office, Ambawadi, Ahmedabad, 380015</t>
   </si>
   <si>
@@ -79,9 +68,6 @@
     <t>Date of Appointment</t>
   </si>
   <si>
-    <t>Company</t>
-  </si>
-  <si>
     <t>Hiten Ramniklal Mehta</t>
   </si>
   <si>
@@ -635,16 +621,25 @@
   </si>
   <si>
     <t>Vasna - Bhayli Main Rd, Near Panchmukhi Hanuman Temple, Vasant Vihar, Bhayli, Vadodara, Gujarat 390015</t>
+  </si>
+  <si>
+    <t>CompanyName</t>
+  </si>
+  <si>
+    <t>SEBIRegistrationNo</t>
+  </si>
+  <si>
+    <t>MemberID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -798,7 +793,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -833,7 +828,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1041,204 +1036,205 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="82.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>6</v>
+        <v>201</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="3" customFormat="1">
       <c r="A2" s="4">
         <v>13233</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:5" s="3" customFormat="1">
       <c r="A3" s="4">
         <v>9098</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:5" s="3" customFormat="1">
       <c r="A4" s="4">
         <v>90039</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="3" customFormat="1">
       <c r="A5" s="4">
         <v>6430</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="3" customFormat="1">
       <c r="A6" s="4">
         <v>12965</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="3" customFormat="1">
       <c r="A7" s="4">
         <v>7701</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="3" customFormat="1">
       <c r="A8" s="4">
         <v>6962</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="3" customFormat="1">
       <c r="A9" s="4">
         <v>8854</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="3" customFormat="1">
       <c r="A10" s="4">
         <v>8256</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="3" customFormat="1">
       <c r="A11" s="4">
         <v>90135</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1248,570 +1244,568 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="2" max="2" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="0" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="9.1640625" customWidth="1"/>
-    <col min="8" max="8" width="34.5" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" customWidth="1"/>
+    <col min="8" max="8" width="34.42578125" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
         <v>17</v>
       </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="B2" t="s">
         <v>15</v>
       </c>
-      <c r="H1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="C2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" t="s">
-        <v>19</v>
-      </c>
       <c r="D2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F2">
         <v>9850364756</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="H2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="I2" s="9">
         <v>39954</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F3">
         <v>9920412896</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H3" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="I3" s="9">
         <v>41341</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F4">
         <v>9821369874</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H4" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="I4" s="9">
         <v>39263</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E5" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F5">
         <v>7048299661</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="H5" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="I5" s="9">
         <v>42771</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F6">
         <v>8433891227</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H6" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="I6" s="9">
         <v>39703</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
         <v>29</v>
       </c>
-      <c r="B7" t="s">
-        <v>32</v>
-      </c>
       <c r="C7" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D7" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F7">
         <v>9932146579</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H7" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="I7" s="9">
         <v>36434</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E8" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F8">
         <v>9874532658</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H8" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="I8" s="9">
         <v>40645</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D9" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E9" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F9">
         <v>9874269745</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H9" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="I9" s="9">
         <v>42233</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s">
         <v>41</v>
       </c>
-      <c r="B10" t="s">
-        <v>44</v>
-      </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E10" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F10">
         <v>9827628450</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H10" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I10" s="9">
         <v>37518</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D11" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E11" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F11">
         <v>9945269873</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H11" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I11" s="9">
         <v>38879</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" t="s">
         <v>48</v>
       </c>
-      <c r="B12" t="s">
-        <v>51</v>
-      </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E12" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F12">
         <v>9876145876</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H12" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="I12" s="9">
         <v>38032</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D13" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E13" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F13">
         <v>9921065394</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H13" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="I13" s="9">
         <v>43814</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="30">
       <c r="A14" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D14" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F14">
         <v>9821065971</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="I14" s="9">
         <v>40187</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="40" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="39">
       <c r="A15" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B15" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D15" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E15" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F15">
         <v>9920563877</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="I15" s="9">
         <v>40915</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B16" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D16" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E16" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F16">
         <v>8665281996</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H16" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="I16" s="9">
         <v>38961</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B17" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C17" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D17" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E17" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F17">
         <v>9821052963</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H17" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="I17" s="9">
         <v>41644</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C18" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D18" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E18" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F18">
         <v>9920746982</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H18" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I18" s="9">
         <v>42373</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B19" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C19" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E19" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F19">
         <v>9827632086</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H19" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="I19" s="9">
         <v>42220</v>
@@ -1843,334 +1837,340 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.5" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="111" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>200</v>
       </c>
       <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" t="s">
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="I1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
-        <v>4</v>
-      </c>
       <c r="B2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F2">
         <v>8046028746</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="H2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="I2" s="8">
         <v>40421</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F3">
         <v>9921057963</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="H3" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I3" s="8">
         <v>41061</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4" s="10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D4" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F4">
         <v>9896732165</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H4" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="I4" s="8">
         <v>40162</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" s="10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C5" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E5" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F5">
         <v>9926452783</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="H5" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="I5" s="8">
         <v>39918</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="A6" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C6" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D6" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E6" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F6">
         <v>8851796475</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="H6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="I6" s="8">
         <v>38353</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9">
       <c r="A7" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C7" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D7" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E7" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F7">
         <v>9821074160</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="H7" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="I7" s="8">
         <v>42139</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9">
       <c r="A8" s="10" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B8" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C8" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D8" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E8" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F8">
         <v>9921055426</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="H8" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="I8" s="8">
         <v>38763</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9">
       <c r="A9" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B9" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C9" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D9" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E9" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F9">
         <v>8477522264</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="H9" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="I9" s="8">
         <v>43282</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9">
       <c r="A10" s="10" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B10" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C10" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D10" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E10" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F10">
         <v>9820565195</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="H10" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="I10" s="8">
         <v>38078</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9">
       <c r="A11" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B11" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C11" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D11" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E11" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F11">
         <v>9973268525</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H11" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="I11" s="8">
         <v>41455</v>

</xml_diff>

<commit_message>
added preliminary new schema python file to gitignore
</commit_message>
<xml_diff>
--- a/server/brokerage_data.xlsx
+++ b/server/brokerage_data.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26215"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tanooj/dynamic_UI/server/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="465" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="20740" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="member_profiles" sheetId="1" r:id="rId1"/>
@@ -21,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="202">
   <si>
     <t>Segments</t>
   </si>
@@ -215,9 +220,6 @@
     <t>C-88, Fourth Floor, Sector 2, Noida, 401301</t>
   </si>
   <si>
-    <t>Quantum Global Securities Ltd</t>
-  </si>
-  <si>
     <t>Atul Narendra Malik</t>
   </si>
   <si>
@@ -623,23 +625,23 @@
     <t>Vasna - Bhayli Main Rd, Near Panchmukhi Hanuman Temple, Vasant Vihar, Bhayli, Vadodara, Gujarat 390015</t>
   </si>
   <si>
-    <t>CompanyName</t>
-  </si>
-  <si>
     <t>SEBIRegistrationNo</t>
   </si>
   <si>
     <t>MemberID</t>
+  </si>
+  <si>
+    <t>MemberName</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1036,38 +1038,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="44" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="82.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="82.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>10</v>
+        <v>201</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="3" customFormat="1">
+    <row r="2" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>13233</v>
       </c>
@@ -1084,7 +1088,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="3" customFormat="1">
+    <row r="3" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>9098</v>
       </c>
@@ -1101,7 +1105,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="3" customFormat="1">
+    <row r="4" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>90039</v>
       </c>
@@ -1118,7 +1122,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="3" customFormat="1">
+    <row r="5" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>6430</v>
       </c>
@@ -1135,7 +1139,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="3" customFormat="1">
+    <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>12965</v>
       </c>
@@ -1152,7 +1156,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="3" customFormat="1">
+    <row r="7" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>7701</v>
       </c>
@@ -1169,7 +1173,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="3" customFormat="1">
+    <row r="8" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>6962</v>
       </c>
@@ -1186,7 +1190,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="3" customFormat="1">
+    <row r="9" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>8854</v>
       </c>
@@ -1203,12 +1207,12 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="3" customFormat="1">
+    <row r="10" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>8256</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>62</v>
@@ -1220,21 +1224,21 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="3" customFormat="1">
+    <row r="11" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>90135</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C11" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="E11" s="5" t="s">
         <v>68</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1244,950 +1248,1042 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B16:B17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="0" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" customWidth="1"/>
-    <col min="8" max="8" width="34.42578125" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="0" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="8" max="8" width="9.1640625" customWidth="1"/>
+    <col min="9" max="9" width="34.5" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>200</v>
       </c>
       <c r="B1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>49</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>2</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="4">
+        <v>9098</v>
+      </c>
+      <c r="B2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>16</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G2">
+        <v>9850364756</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="I2" t="s">
+        <v>171</v>
+      </c>
+      <c r="J2" s="9">
+        <v>39954</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
+        <v>9098</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
         <v>109</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F3" t="s">
         <v>91</v>
       </c>
-      <c r="F2">
-        <v>9850364756</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="G3">
+        <v>9920412896</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I3" t="s">
         <v>172</v>
       </c>
-      <c r="I2" s="9">
-        <v>39954</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="J3" s="9">
+        <v>41341</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>13233</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
         <v>19</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E4" t="s">
         <v>110</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F4" t="s">
         <v>92</v>
       </c>
-      <c r="F3">
-        <v>9920412896</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="G4">
+        <v>9821369874</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I4" t="s">
+        <v>182</v>
+      </c>
+      <c r="J4" s="9">
+        <v>39263</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>13233</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" t="s">
+        <v>111</v>
+      </c>
+      <c r="F5" t="s">
+        <v>93</v>
+      </c>
+      <c r="G5">
+        <v>7048299661</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I5" t="s">
+        <v>183</v>
+      </c>
+      <c r="J5" s="9">
+        <v>42771</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
+        <v>90039</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F6" t="s">
+        <v>94</v>
+      </c>
+      <c r="G6">
+        <v>8433891227</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I6" t="s">
+        <v>184</v>
+      </c>
+      <c r="J6" s="9">
+        <v>39703</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <v>90039</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F7" t="s">
+        <v>95</v>
+      </c>
+      <c r="G7">
+        <v>9932146579</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I7" t="s">
+        <v>185</v>
+      </c>
+      <c r="J7" s="9">
+        <v>36434</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
+        <v>6430</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" t="s">
+        <v>114</v>
+      </c>
+      <c r="F8" t="s">
+        <v>96</v>
+      </c>
+      <c r="G8">
+        <v>9874532658</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I8" t="s">
+        <v>186</v>
+      </c>
+      <c r="J8" s="9">
+        <v>40645</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="4">
+        <v>12965</v>
+      </c>
+      <c r="B9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" t="s">
+        <v>115</v>
+      </c>
+      <c r="F9" t="s">
+        <v>97</v>
+      </c>
+      <c r="G9">
+        <v>9874269745</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I9" t="s">
+        <v>191</v>
+      </c>
+      <c r="J9" s="9">
+        <v>42233</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
+        <v>12965</v>
+      </c>
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" t="s">
+        <v>116</v>
+      </c>
+      <c r="F10" t="s">
+        <v>98</v>
+      </c>
+      <c r="G10">
+        <v>9827628450</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I10" t="s">
+        <v>192</v>
+      </c>
+      <c r="J10" s="9">
+        <v>37518</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="4">
+        <v>7701</v>
+      </c>
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" t="s">
+        <v>117</v>
+      </c>
+      <c r="F11" t="s">
+        <v>99</v>
+      </c>
+      <c r="G11">
+        <v>9945269873</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I11" t="s">
+        <v>187</v>
+      </c>
+      <c r="J11" s="9">
+        <v>38879</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
+        <v>7701</v>
+      </c>
+      <c r="B12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" t="s">
+        <v>118</v>
+      </c>
+      <c r="F12" t="s">
+        <v>100</v>
+      </c>
+      <c r="G12">
+        <v>9876145876</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I12" t="s">
+        <v>188</v>
+      </c>
+      <c r="J12" s="9">
+        <v>38032</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="4">
+        <v>6962</v>
+      </c>
+      <c r="B13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" t="s">
+        <v>119</v>
+      </c>
+      <c r="F13" t="s">
+        <v>101</v>
+      </c>
+      <c r="G13">
+        <v>9921065394</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I13" t="s">
+        <v>198</v>
+      </c>
+      <c r="J13" s="9">
+        <v>43814</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="A14" s="4">
+        <v>8854</v>
+      </c>
+      <c r="B14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" t="s">
+        <v>120</v>
+      </c>
+      <c r="F14" t="s">
+        <v>102</v>
+      </c>
+      <c r="G14">
+        <v>9821065971</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I14" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="I3" s="9">
-        <v>41341</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>111</v>
-      </c>
-      <c r="E4" t="s">
-        <v>93</v>
-      </c>
-      <c r="F4">
-        <v>9821369874</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="H4" t="s">
-        <v>183</v>
-      </c>
-      <c r="I4" s="9">
-        <v>39263</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="J14" s="9">
+        <v>40187</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="40" x14ac:dyDescent="0.2">
+      <c r="A15" s="4">
+        <v>8854</v>
+      </c>
+      <c r="B15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" t="s">
+        <v>121</v>
+      </c>
+      <c r="F15" t="s">
+        <v>103</v>
+      </c>
+      <c r="G15">
+        <v>9920563877</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="J15" s="9">
+        <v>40915</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="4">
+        <v>8256</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="C16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" t="s">
         <v>28</v>
       </c>
-      <c r="D5" t="s">
-        <v>112</v>
-      </c>
-      <c r="E5" t="s">
-        <v>94</v>
-      </c>
-      <c r="F5">
-        <v>7048299661</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="H5" t="s">
-        <v>184</v>
-      </c>
-      <c r="I5" s="9">
-        <v>42771</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" t="s">
-        <v>113</v>
-      </c>
-      <c r="E6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F6">
-        <v>8433891227</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="H6" t="s">
-        <v>185</v>
-      </c>
-      <c r="I6" s="9">
-        <v>39703</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="E16" t="s">
+        <v>122</v>
+      </c>
+      <c r="F16" t="s">
+        <v>104</v>
+      </c>
+      <c r="G16">
+        <v>8665281996</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I16" t="s">
+        <v>195</v>
+      </c>
+      <c r="J16" s="9">
+        <v>38961</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="4">
+        <v>8256</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="C17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" t="s">
         <v>127</v>
       </c>
-      <c r="D7" t="s">
-        <v>114</v>
-      </c>
-      <c r="E7" t="s">
-        <v>96</v>
-      </c>
-      <c r="F7">
-        <v>9932146579</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H7" t="s">
-        <v>186</v>
-      </c>
-      <c r="I7" s="9">
-        <v>36434</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" t="s">
-        <v>115</v>
-      </c>
-      <c r="E8" t="s">
-        <v>97</v>
-      </c>
-      <c r="F8">
-        <v>9874532658</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="H8" t="s">
-        <v>187</v>
-      </c>
-      <c r="I8" s="9">
-        <v>40645</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="E17" t="s">
+        <v>123</v>
+      </c>
+      <c r="F17" t="s">
+        <v>105</v>
+      </c>
+      <c r="G17">
+        <v>9821052963</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I17" t="s">
+        <v>196</v>
+      </c>
+      <c r="J17" s="9">
+        <v>41644</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="4">
+        <v>90135</v>
+      </c>
+      <c r="B18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" t="s">
         <v>40</v>
       </c>
-      <c r="D9" t="s">
-        <v>116</v>
-      </c>
-      <c r="E9" t="s">
-        <v>98</v>
-      </c>
-      <c r="F9">
-        <v>9874269745</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="H9" t="s">
-        <v>192</v>
-      </c>
-      <c r="I9" s="9">
-        <v>42233</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="E18" t="s">
+        <v>124</v>
+      </c>
+      <c r="F18" t="s">
+        <v>106</v>
+      </c>
+      <c r="G18">
+        <v>9920746982</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I18" t="s">
+        <v>176</v>
+      </c>
+      <c r="J18" s="9">
+        <v>42373</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="4">
+        <v>90135</v>
+      </c>
+      <c r="B19" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19" t="s">
         <v>16</v>
       </c>
-      <c r="D10" t="s">
-        <v>117</v>
-      </c>
-      <c r="E10" t="s">
-        <v>99</v>
-      </c>
-      <c r="F10">
-        <v>9827628450</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="H10" t="s">
-        <v>193</v>
-      </c>
-      <c r="I10" s="9">
-        <v>37518</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C11" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" t="s">
-        <v>118</v>
-      </c>
-      <c r="E11" t="s">
-        <v>100</v>
-      </c>
-      <c r="F11">
-        <v>9945269873</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="H11" t="s">
-        <v>188</v>
-      </c>
-      <c r="I11" s="9">
-        <v>38879</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" t="s">
-        <v>119</v>
-      </c>
-      <c r="E12" t="s">
-        <v>101</v>
-      </c>
-      <c r="F12">
-        <v>9876145876</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="H12" t="s">
-        <v>189</v>
-      </c>
-      <c r="I12" s="9">
-        <v>38032</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" t="s">
-        <v>53</v>
-      </c>
-      <c r="B13" t="s">
-        <v>54</v>
-      </c>
-      <c r="C13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" t="s">
-        <v>120</v>
-      </c>
-      <c r="E13" t="s">
-        <v>102</v>
-      </c>
-      <c r="F13">
-        <v>9921065394</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="H13" t="s">
-        <v>199</v>
-      </c>
-      <c r="I13" s="9">
-        <v>43814</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="30">
-      <c r="A14" t="s">
-        <v>58</v>
-      </c>
-      <c r="B14" t="s">
-        <v>59</v>
-      </c>
-      <c r="C14" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" t="s">
-        <v>121</v>
-      </c>
-      <c r="E14" t="s">
-        <v>103</v>
-      </c>
-      <c r="F14">
-        <v>9821065971</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H14" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="I14" s="9">
-        <v>40187</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="39">
-      <c r="A15" t="s">
-        <v>58</v>
-      </c>
-      <c r="B15" t="s">
-        <v>60</v>
-      </c>
-      <c r="C15" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" t="s">
-        <v>122</v>
-      </c>
-      <c r="E15" t="s">
-        <v>104</v>
-      </c>
-      <c r="F15">
-        <v>9920563877</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="H15" s="11" t="s">
+      <c r="E19" t="s">
+        <v>125</v>
+      </c>
+      <c r="F19" t="s">
+        <v>107</v>
+      </c>
+      <c r="G19">
+        <v>9827632086</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I19" t="s">
         <v>175</v>
       </c>
-      <c r="I15" s="9">
-        <v>40915</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" t="s">
-        <v>64</v>
-      </c>
-      <c r="B16" t="s">
-        <v>65</v>
-      </c>
-      <c r="C16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" t="s">
-        <v>123</v>
-      </c>
-      <c r="E16" t="s">
-        <v>105</v>
-      </c>
-      <c r="F16">
-        <v>8665281996</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H16" t="s">
-        <v>196</v>
-      </c>
-      <c r="I16" s="9">
-        <v>38961</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" t="s">
-        <v>64</v>
-      </c>
-      <c r="B17" t="s">
-        <v>66</v>
-      </c>
-      <c r="C17" t="s">
-        <v>128</v>
-      </c>
-      <c r="D17" t="s">
-        <v>124</v>
-      </c>
-      <c r="E17" t="s">
-        <v>106</v>
-      </c>
-      <c r="F17">
-        <v>9821052963</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="H17" t="s">
-        <v>197</v>
-      </c>
-      <c r="I17" s="9">
-        <v>41644</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" t="s">
-        <v>70</v>
-      </c>
-      <c r="B18" t="s">
-        <v>71</v>
-      </c>
-      <c r="C18" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" t="s">
-        <v>125</v>
-      </c>
-      <c r="E18" t="s">
-        <v>107</v>
-      </c>
-      <c r="F18">
-        <v>9920746982</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="H18" t="s">
-        <v>177</v>
-      </c>
-      <c r="I18" s="9">
-        <v>42373</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" t="s">
-        <v>70</v>
-      </c>
-      <c r="B19" t="s">
-        <v>72</v>
-      </c>
-      <c r="C19" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" t="s">
-        <v>126</v>
-      </c>
-      <c r="E19" t="s">
-        <v>108</v>
-      </c>
-      <c r="F19">
-        <v>9827632086</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="H19" t="s">
-        <v>176</v>
-      </c>
-      <c r="I19" s="9">
+      <c r="J19" s="9">
         <v>42220</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G19" r:id="rId1"/>
-    <hyperlink ref="G18" r:id="rId2"/>
-    <hyperlink ref="G17" r:id="rId3"/>
-    <hyperlink ref="G16" r:id="rId4"/>
-    <hyperlink ref="G15" r:id="rId5"/>
-    <hyperlink ref="G14" r:id="rId6"/>
-    <hyperlink ref="G13" r:id="rId7"/>
-    <hyperlink ref="G12" r:id="rId8"/>
-    <hyperlink ref="G11" r:id="rId9"/>
-    <hyperlink ref="G10" r:id="rId10"/>
-    <hyperlink ref="G9" r:id="rId11"/>
-    <hyperlink ref="G8" r:id="rId12"/>
-    <hyperlink ref="G7" r:id="rId13"/>
-    <hyperlink ref="G6" r:id="rId14"/>
-    <hyperlink ref="G5" r:id="rId15"/>
-    <hyperlink ref="G4" r:id="rId16"/>
-    <hyperlink ref="G3" r:id="rId17"/>
-    <hyperlink ref="G2" r:id="rId18"/>
+    <hyperlink ref="H19" r:id="rId1"/>
+    <hyperlink ref="H18" r:id="rId2"/>
+    <hyperlink ref="H17" r:id="rId3"/>
+    <hyperlink ref="H16" r:id="rId4"/>
+    <hyperlink ref="H15" r:id="rId5"/>
+    <hyperlink ref="H14" r:id="rId6"/>
+    <hyperlink ref="H13" r:id="rId7"/>
+    <hyperlink ref="H12" r:id="rId8"/>
+    <hyperlink ref="H11" r:id="rId9"/>
+    <hyperlink ref="H10" r:id="rId10"/>
+    <hyperlink ref="H9" r:id="rId11"/>
+    <hyperlink ref="H8" r:id="rId12"/>
+    <hyperlink ref="H7" r:id="rId13"/>
+    <hyperlink ref="H6" r:id="rId14"/>
+    <hyperlink ref="H5" r:id="rId15"/>
+    <hyperlink ref="H4" r:id="rId16"/>
+    <hyperlink ref="H3" r:id="rId17"/>
+    <hyperlink ref="H2" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="111" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="111" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>200</v>
       </c>
       <c r="B1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>49</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>2</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="4">
+        <v>13233</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G2">
+        <v>8046028746</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="I2" t="s">
+        <v>180</v>
+      </c>
+      <c r="J2" s="8">
+        <v>40421</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
+        <v>9098</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
         <v>150</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D3" t="s">
         <v>170</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E3" t="s">
         <v>140</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F3" t="s">
         <v>130</v>
       </c>
-      <c r="F2">
-        <v>8046028746</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="G3">
+        <v>9921057963</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I3" t="s">
+        <v>177</v>
+      </c>
+      <c r="J3" s="8">
+        <v>41061</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>90039</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D4" t="s">
+        <v>169</v>
+      </c>
+      <c r="E4" t="s">
+        <v>141</v>
+      </c>
+      <c r="F4" t="s">
+        <v>131</v>
+      </c>
+      <c r="G4">
+        <v>9896732165</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I4" t="s">
         <v>181</v>
       </c>
-      <c r="I2" s="8">
-        <v>40421</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" t="s">
-        <v>151</v>
-      </c>
-      <c r="C3" t="s">
-        <v>171</v>
-      </c>
-      <c r="D3" t="s">
-        <v>141</v>
-      </c>
-      <c r="E3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F3">
-        <v>9921057963</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="J4" s="8">
+        <v>40162</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>6430</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>152</v>
+      </c>
+      <c r="D5" t="s">
+        <v>169</v>
+      </c>
+      <c r="E5" t="s">
+        <v>142</v>
+      </c>
+      <c r="F5" t="s">
+        <v>132</v>
+      </c>
+      <c r="G5">
+        <v>9926452783</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I5" t="s">
+        <v>189</v>
+      </c>
+      <c r="J5" s="8">
+        <v>39918</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
+        <v>12965</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" t="s">
+        <v>153</v>
+      </c>
+      <c r="D6" t="s">
+        <v>170</v>
+      </c>
+      <c r="E6" t="s">
+        <v>143</v>
+      </c>
+      <c r="F6" t="s">
+        <v>133</v>
+      </c>
+      <c r="G6">
+        <v>8851796475</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="I6" t="s">
+        <v>193</v>
+      </c>
+      <c r="J6" s="8">
+        <v>38353</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <v>7701</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" t="s">
+        <v>154</v>
+      </c>
+      <c r="D7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E7" t="s">
+        <v>144</v>
+      </c>
+      <c r="F7" t="s">
+        <v>134</v>
+      </c>
+      <c r="G7">
+        <v>9821074160</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="I7" t="s">
+        <v>190</v>
+      </c>
+      <c r="J7" s="8">
+        <v>42139</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
+        <v>6962</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D8" t="s">
+        <v>126</v>
+      </c>
+      <c r="E8" t="s">
+        <v>145</v>
+      </c>
+      <c r="F8" t="s">
+        <v>135</v>
+      </c>
+      <c r="G8">
+        <v>9921055426</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="I8" t="s">
+        <v>197</v>
+      </c>
+      <c r="J8" s="8">
+        <v>38763</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="4">
+        <v>8854</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" t="s">
+        <v>156</v>
+      </c>
+      <c r="D9" t="s">
+        <v>169</v>
+      </c>
+      <c r="E9" t="s">
+        <v>146</v>
+      </c>
+      <c r="F9" t="s">
+        <v>136</v>
+      </c>
+      <c r="G9">
+        <v>8477522264</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="I9" t="s">
         <v>178</v>
       </c>
-      <c r="I3" s="8">
-        <v>41061</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" t="s">
-        <v>152</v>
-      </c>
-      <c r="C4" t="s">
-        <v>170</v>
-      </c>
-      <c r="D4" t="s">
-        <v>142</v>
-      </c>
-      <c r="E4" t="s">
-        <v>132</v>
-      </c>
-      <c r="F4">
-        <v>9896732165</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="H4" t="s">
-        <v>182</v>
-      </c>
-      <c r="I4" s="8">
-        <v>40162</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" t="s">
-        <v>153</v>
-      </c>
-      <c r="C5" t="s">
-        <v>170</v>
-      </c>
-      <c r="D5" t="s">
-        <v>143</v>
-      </c>
-      <c r="E5" t="s">
-        <v>133</v>
-      </c>
-      <c r="F5">
-        <v>9926452783</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="H5" t="s">
-        <v>190</v>
-      </c>
-      <c r="I5" s="8">
-        <v>39918</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" t="s">
-        <v>154</v>
-      </c>
-      <c r="C6" t="s">
-        <v>171</v>
-      </c>
-      <c r="D6" t="s">
-        <v>144</v>
-      </c>
-      <c r="E6" t="s">
-        <v>134</v>
-      </c>
-      <c r="F6">
-        <v>8851796475</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="H6" t="s">
+      <c r="J9" s="8">
+        <v>43282</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
+        <v>8256</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="C10" t="s">
+        <v>157</v>
+      </c>
+      <c r="D10" t="s">
+        <v>169</v>
+      </c>
+      <c r="E10" t="s">
+        <v>147</v>
+      </c>
+      <c r="F10" t="s">
+        <v>137</v>
+      </c>
+      <c r="G10">
+        <v>9820565195</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="I10" t="s">
         <v>194</v>
       </c>
-      <c r="I6" s="8">
-        <v>38353</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7" t="s">
-        <v>155</v>
-      </c>
-      <c r="C7" t="s">
-        <v>170</v>
-      </c>
-      <c r="D7" t="s">
-        <v>145</v>
-      </c>
-      <c r="E7" t="s">
-        <v>135</v>
-      </c>
-      <c r="F7">
-        <v>9821074160</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="H7" t="s">
-        <v>191</v>
-      </c>
-      <c r="I7" s="8">
-        <v>42139</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" t="s">
-        <v>156</v>
-      </c>
-      <c r="C8" t="s">
-        <v>127</v>
-      </c>
-      <c r="D8" t="s">
-        <v>146</v>
-      </c>
-      <c r="E8" t="s">
-        <v>136</v>
-      </c>
-      <c r="F8">
-        <v>9921055426</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="H8" t="s">
-        <v>198</v>
-      </c>
-      <c r="I8" s="8">
-        <v>38763</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B9" t="s">
-        <v>157</v>
-      </c>
-      <c r="C9" t="s">
-        <v>170</v>
-      </c>
-      <c r="D9" t="s">
-        <v>147</v>
-      </c>
-      <c r="E9" t="s">
-        <v>137</v>
-      </c>
-      <c r="F9">
-        <v>8477522264</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="H9" t="s">
+      <c r="J10" s="8">
+        <v>38078</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="4">
+        <v>90135</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" t="s">
+        <v>158</v>
+      </c>
+      <c r="D11" t="s">
+        <v>169</v>
+      </c>
+      <c r="E11" t="s">
+        <v>148</v>
+      </c>
+      <c r="F11" t="s">
+        <v>138</v>
+      </c>
+      <c r="G11">
+        <v>9973268525</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="I11" t="s">
         <v>179</v>
       </c>
-      <c r="I9" s="8">
-        <v>43282</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="B10" t="s">
-        <v>158</v>
-      </c>
-      <c r="C10" t="s">
-        <v>170</v>
-      </c>
-      <c r="D10" t="s">
-        <v>148</v>
-      </c>
-      <c r="E10" t="s">
-        <v>138</v>
-      </c>
-      <c r="F10">
-        <v>9820565195</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="H10" t="s">
-        <v>195</v>
-      </c>
-      <c r="I10" s="8">
-        <v>38078</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B11" t="s">
-        <v>159</v>
-      </c>
-      <c r="C11" t="s">
-        <v>170</v>
-      </c>
-      <c r="D11" t="s">
-        <v>149</v>
-      </c>
-      <c r="E11" t="s">
-        <v>139</v>
-      </c>
-      <c r="F11">
-        <v>9973268525</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="H11" t="s">
-        <v>180</v>
-      </c>
-      <c r="I11" s="8">
+      <c r="J11" s="8">
         <v>41455</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="G3" r:id="rId2"/>
-    <hyperlink ref="G4" r:id="rId3"/>
-    <hyperlink ref="G5" r:id="rId4"/>
-    <hyperlink ref="G6" r:id="rId5"/>
-    <hyperlink ref="G7" r:id="rId6"/>
-    <hyperlink ref="G8" r:id="rId7"/>
-    <hyperlink ref="G9" r:id="rId8"/>
-    <hyperlink ref="G10" r:id="rId9"/>
-    <hyperlink ref="G11" r:id="rId10"/>
+    <hyperlink ref="H2" r:id="rId1"/>
+    <hyperlink ref="H3" r:id="rId2"/>
+    <hyperlink ref="H4" r:id="rId3"/>
+    <hyperlink ref="H5" r:id="rId4"/>
+    <hyperlink ref="H6" r:id="rId5"/>
+    <hyperlink ref="H7" r:id="rId6"/>
+    <hyperlink ref="H8" r:id="rId7"/>
+    <hyperlink ref="H9" r:id="rId8"/>
+    <hyperlink ref="H10" r:id="rId9"/>
+    <hyperlink ref="H11" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>